<commit_message>
Exo partie 4 logic
</commit_message>
<xml_diff>
--- a/Intro_AI/Exo Logique 3.xlsx
+++ b/Intro_AI/Exo Logique 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\M1_DSC\Intro_AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{352E97E6-C130-4723-89FD-E27E619650C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EF12EC-E1B8-4752-AD58-9BA4B65AE31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{51786762-2B49-4CF6-81E0-FB50EDF694E0}"/>
+    <workbookView minimized="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{51786762-2B49-4CF6-81E0-FB50EDF694E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1168,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BE9696-AD8A-49CC-B53F-20E827B66154}">
   <dimension ref="B3:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>